<commit_message>
Before removing the old 3-row figure
</commit_message>
<xml_diff>
--- a/csvs/convergence_check.xlsx
+++ b/csvs/convergence_check.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="SingleElem" sheetId="1" r:id="rId1"/>
-    <sheet name="Artery" sheetId="2" r:id="rId2"/>
+    <sheet name="Prez" sheetId="3" r:id="rId2"/>
+    <sheet name="Artery" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
-  <si>
-    <t>Numeric</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="20">
   <si>
     <t>Analytic</t>
   </si>
@@ -82,6 +80,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Radius rel. err.</t>
+  </si>
+  <si>
+    <t>Numerical</t>
   </si>
 </sst>
 </file>
@@ -141,14 +145,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -158,6 +159,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B10:Y34"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -463,137 +476,137 @@
   <sheetData>
     <row r="10" spans="2:22">
       <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4" t="s">
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
     </row>
     <row r="11" spans="2:22">
       <c r="B11" s="1"/>
-      <c r="C11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4"/>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K11" s="4"/>
+      <c r="H11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P11" s="4"/>
+      <c r="M11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="8"/>
       <c r="Q11" s="3"/>
-      <c r="R11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="U11" s="4"/>
+      <c r="R11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="U11" s="8"/>
       <c r="V11" s="3"/>
     </row>
     <row r="12" spans="2:22">
       <c r="B12" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="H12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="J12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="M12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="O12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="R12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="T12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V12" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:22">
@@ -714,7 +727,7 @@
         <v>187278</v>
       </c>
       <c r="Q14" s="2">
-        <f t="shared" ref="Q14:Q34" si="2">ABS((N14-P14)/P14)</f>
+        <f t="shared" ref="Q14:Q32" si="2">ABS((N14-P14)/P14)</f>
         <v>1.4951035359198625E-4</v>
       </c>
       <c r="R14" s="1">
@@ -730,7 +743,7 @@
         <v>15994</v>
       </c>
       <c r="V14" s="2">
-        <f t="shared" ref="V14:V34" si="3">ABS((S14-U14)/U14)</f>
+        <f t="shared" ref="V14:V32" si="3">ABS((S14-U14)/U14)</f>
         <v>1.2504689258517419E-5</v>
       </c>
     </row>
@@ -1978,13 +1991,13 @@
     </row>
     <row r="33" spans="2:25">
       <c r="B33" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="5">
+      <c r="G33" s="4">
         <f>AVERAGE(G13:G32)</f>
         <v>1.6904768999307886E-4</v>
       </c>
@@ -1992,7 +2005,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="5">
+      <c r="L33" s="4">
         <f>AVERAGE(L13:L32)</f>
         <v>5.2039948416438715E-5</v>
       </c>
@@ -2000,7 +2013,7 @@
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
-      <c r="Q33" s="5">
+      <c r="Q33" s="4">
         <f>AVERAGE(Q13:Q32)</f>
         <v>5.5428514568710733E-5</v>
       </c>
@@ -2008,7 +2021,7 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
-      <c r="V33" s="5">
+      <c r="V33" s="4">
         <f>AVERAGE(V13:V32)</f>
         <v>1.5792689970088683E-5</v>
       </c>
@@ -2019,7 +2032,7 @@
     </row>
     <row r="34" spans="2:25">
       <c r="B34" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C34" s="3">
         <f>SUM(C13:C32)</f>
@@ -2068,6 +2081,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="M10:Q10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
     <mergeCell ref="R10:V10"/>
     <mergeCell ref="R11:S11"/>
     <mergeCell ref="T11:U11"/>
@@ -2075,11 +2093,6 @@
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="O11:P11"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="M10:Q10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2088,10 +2101,225 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7">
+      <c r="B3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="9">
+        <v>22</v>
+      </c>
+      <c r="C6" s="9">
+        <v>21</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1.6904768999307886E-4</v>
+      </c>
+      <c r="E6" s="9">
+        <v>27</v>
+      </c>
+      <c r="F6" s="9">
+        <v>25</v>
+      </c>
+      <c r="G6" s="11">
+        <v>5.2039948416438715E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="9">
+        <v>41</v>
+      </c>
+      <c r="C10" s="9">
+        <v>41</v>
+      </c>
+      <c r="D10" s="11">
+        <v>5.5428514568710733E-5</v>
+      </c>
+      <c r="E10" s="9">
+        <v>21</v>
+      </c>
+      <c r="F10" s="9">
+        <v>21</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1.5792689970088683E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="C12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="C13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="C14" s="9">
+        <v>9</v>
+      </c>
+      <c r="D14" s="9">
+        <v>30</v>
+      </c>
+      <c r="E14" s="9">
+        <v>8</v>
+      </c>
+      <c r="F14" s="9">
+        <v>40</v>
+      </c>
+      <c r="G14" s="11">
+        <v>4.2507970244070097E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2106,10 +2334,10 @@
   <sheetData>
     <row r="1" spans="2:12">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="2:12">
@@ -2117,7 +2345,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2132,7 +2360,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -2213,7 +2441,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2228,7 +2456,7 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -2386,290 +2614,290 @@
       </c>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="J14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="K14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="8" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="6">
-        <v>1</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1</v>
+      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5">
+        <v>4</v>
+      </c>
+      <c r="E16" s="6">
+        <v>6.25</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.45727869999999998</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="H16" s="5">
+        <v>2</v>
+      </c>
+      <c r="I16" s="5">
+        <v>4</v>
+      </c>
+      <c r="J16" s="6">
+        <v>6.25</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0.45727899999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.62967300000000004</v>
+      </c>
+      <c r="G17" s="5">
+        <v>2</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1</v>
+      </c>
+      <c r="I17" s="5">
+        <v>8</v>
+      </c>
+      <c r="J17" s="6">
+        <v>12.5</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0.62967399999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="5">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="5">
+        <v>3</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="5">
+        <v>9</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="B19" s="5">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2</v>
+      </c>
+      <c r="D19" s="5">
         <v>6</v>
       </c>
-      <c r="D15" s="6">
-        <v>1</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6">
-        <v>1</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="E19" s="6">
+        <v>14.84375</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.65888000000000002</v>
+      </c>
+      <c r="G19" s="5">
+        <v>3</v>
+      </c>
+      <c r="H19" s="5">
+        <v>2</v>
+      </c>
+      <c r="I19" s="5">
+        <v>9</v>
+      </c>
+      <c r="J19" s="6">
+        <v>15.625</v>
+      </c>
+      <c r="K19" s="6">
+        <v>0.66500100000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="B20" s="5">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
+        <v>4</v>
+      </c>
+      <c r="E20" s="6">
+        <v>17.1875</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.67490400000000006</v>
+      </c>
+      <c r="G20" s="5">
+        <v>4</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1</v>
+      </c>
+      <c r="I20" s="5">
+        <v>4</v>
+      </c>
+      <c r="J20" s="6">
+        <v>18.75</v>
+      </c>
+      <c r="K20" s="6">
+        <v>0.68286999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="5">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5">
+        <v>3</v>
+      </c>
+      <c r="E21" s="6">
+        <v>19.53125</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.68636900000000001</v>
+      </c>
+      <c r="G21" s="5">
+        <v>5</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5">
+        <v>3</v>
+      </c>
+      <c r="J21" s="6">
+        <v>21.875</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0.69555599999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22" s="5">
         <v>6</v>
       </c>
-      <c r="I15" s="6">
-        <v>1</v>
-      </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="2:12">
-      <c r="B16" s="6">
-        <v>1</v>
-      </c>
-      <c r="C16" s="6">
-        <v>2</v>
-      </c>
-      <c r="D16" s="6">
-        <v>4</v>
-      </c>
-      <c r="E16" s="7">
-        <v>6.25</v>
-      </c>
-      <c r="F16" s="7">
-        <v>0.45727869999999998</v>
-      </c>
-      <c r="G16" s="6">
-        <v>1</v>
-      </c>
-      <c r="H16" s="6">
-        <v>2</v>
-      </c>
-      <c r="I16" s="6">
-        <v>4</v>
-      </c>
-      <c r="J16" s="7">
-        <v>6.25</v>
-      </c>
-      <c r="K16" s="7">
-        <v>0.45727899999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12">
-      <c r="B17" s="6">
-        <v>2</v>
-      </c>
-      <c r="C17" s="6">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6">
-        <v>4</v>
-      </c>
-      <c r="E17" s="7">
-        <v>12.5</v>
-      </c>
-      <c r="F17" s="7">
-        <v>0.62967300000000004</v>
-      </c>
-      <c r="G17" s="6">
-        <v>2</v>
-      </c>
-      <c r="H17" s="6">
-        <v>1</v>
-      </c>
-      <c r="I17" s="6">
-        <v>8</v>
-      </c>
-      <c r="J17" s="7">
-        <v>12.5</v>
-      </c>
-      <c r="K17" s="7">
-        <v>0.62967399999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12">
-      <c r="B18" s="6">
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5">
         <v>3</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="E22" s="6">
+        <v>23.046875</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.69959800000000005</v>
+      </c>
+      <c r="G22" s="5">
         <v>6</v>
       </c>
-      <c r="D18" s="6">
-        <v>3</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="6">
-        <v>3</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="6">
-        <v>9</v>
-      </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-    </row>
-    <row r="19" spans="2:12">
-      <c r="B19" s="6">
-        <v>3</v>
-      </c>
-      <c r="C19" s="6">
-        <v>2</v>
-      </c>
-      <c r="D19" s="6">
-        <v>6</v>
-      </c>
-      <c r="E19" s="7">
-        <v>14.84375</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0.65888000000000002</v>
-      </c>
-      <c r="G19" s="6">
-        <v>3</v>
-      </c>
-      <c r="H19" s="6">
-        <v>2</v>
-      </c>
-      <c r="I19" s="6">
-        <v>9</v>
-      </c>
-      <c r="J19" s="7">
-        <v>15.625</v>
-      </c>
-      <c r="K19" s="7">
-        <v>0.66500100000000006</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12">
-      <c r="B20" s="6">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6">
-        <v>1</v>
-      </c>
-      <c r="D20" s="6">
-        <v>4</v>
-      </c>
-      <c r="E20" s="7">
-        <v>17.1875</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0.67490400000000006</v>
-      </c>
-      <c r="G20" s="6">
-        <v>4</v>
-      </c>
-      <c r="H20" s="6">
-        <v>1</v>
-      </c>
-      <c r="I20" s="6">
-        <v>4</v>
-      </c>
-      <c r="J20" s="7">
-        <v>18.75</v>
-      </c>
-      <c r="K20" s="7">
-        <v>0.68286999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12">
-      <c r="B21" s="6">
-        <v>5</v>
-      </c>
-      <c r="C21" s="6">
-        <v>1</v>
-      </c>
-      <c r="D21" s="6">
-        <v>3</v>
-      </c>
-      <c r="E21" s="7">
-        <v>19.53125</v>
-      </c>
-      <c r="F21" s="7">
-        <v>0.68636900000000001</v>
-      </c>
-      <c r="G21" s="6">
-        <v>5</v>
-      </c>
-      <c r="H21" s="6">
-        <v>1</v>
-      </c>
-      <c r="I21" s="6">
-        <v>3</v>
-      </c>
-      <c r="J21" s="7">
-        <v>21.875</v>
-      </c>
-      <c r="K21" s="7">
-        <v>0.69555599999999995</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
-      <c r="B22" s="6">
-        <v>6</v>
-      </c>
-      <c r="C22" s="6">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6">
-        <v>3</v>
-      </c>
-      <c r="E22" s="7">
-        <v>23.046875</v>
-      </c>
-      <c r="F22" s="7">
-        <v>0.69959800000000005</v>
-      </c>
-      <c r="G22" s="6">
-        <v>6</v>
-      </c>
-      <c r="H22" s="6">
-        <v>1</v>
-      </c>
-      <c r="I22" s="6">
-        <v>2</v>
-      </c>
-      <c r="J22" s="7">
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22" s="5">
+        <v>2</v>
+      </c>
+      <c r="J22" s="6">
         <v>25</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="6">
         <v>0.70574999999999999</v>
       </c>
       <c r="L22">
@@ -2678,52 +2906,52 @@
       </c>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>7</v>
       </c>
-      <c r="C23" s="6">
-        <v>1</v>
-      </c>
-      <c r="D23" s="6">
-        <v>2</v>
-      </c>
-      <c r="E23" s="7">
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2</v>
+      </c>
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>0.70574700000000001</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="8">
-        <f>COUNT(C15:C23)</f>
-        <v>7</v>
-      </c>
-      <c r="D24" s="8">
+      <c r="B24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="7">
+        <f>COUNTA(C15:C23)</f>
+        <v>9</v>
+      </c>
+      <c r="D24" s="7">
         <f>SUM(D15:D23)</f>
         <v>30</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8">
-        <f>COUNT(H15:H23)</f>
-        <v>6</v>
-      </c>
-      <c r="I24" s="8">
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7">
+        <f>COUNTA(H15:H23)</f>
+        <v>8</v>
+      </c>
+      <c r="I24" s="7">
         <f>SUM(I15:I23)</f>
         <v>40</v>
       </c>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>